<commit_message>
added jupyter notebook and updated report
</commit_message>
<xml_diff>
--- a/assignment3/Evaluation result.xlsx
+++ b/assignment3/Evaluation result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dil\2020-1학기\학부수업(데이터과학)\과제3.CIFAR-10\CIFAR10-assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimmy\Desktop\Wiles\School\2020\DSc\Github\COSE471\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D478925F-BB7B-4A1B-887F-81D197E08819}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9667339-770F-459A-BDD5-4B5D85E7C5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>CIFAR-10 Evaluation Report</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>Batch_size</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
   </si>
   <si>
     <t>Validation dataset accuracy plot</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [결과 정리]</t>
   </si>
   <si>
     <t>Activation function</t>
@@ -106,23 +100,108 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Lenet5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>ResNet32</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>GPU(O/X)</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>He_normal</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>N.A.</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">36.21 (without </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>val_acc storage)</t>
+    </r>
+  </si>
+  <si>
+    <t>140.49</t>
+  </si>
+  <si>
+    <t>46.40%</t>
+  </si>
+  <si>
+    <t>89.24%</t>
+  </si>
+  <si>
+    <t>Setting #4</t>
+  </si>
+  <si>
+    <t>10.00%</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Model(s)</t>
+  </si>
+  <si>
+    <t>LeNet5</t>
+  </si>
+  <si>
+    <t>X (LeNet5) / He_normal (MLP, ResNet 32)</t>
+  </si>
+  <si>
+    <t>N.A. (training stopped prematurely)</t>
+  </si>
+  <si>
+    <t>N.A (training stopped prematurely)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [결과 정리] To accelerate training, the code provided was modified to run on Google Colab. In fact, it was approximately 6 times faster than using the GPU originally owned (it took &gt;7 hours to train ResNet32 on the personal GPU), although the addition of file-saving procedures (i.e. val_acc storage) slowed the code down considerably (since drive access using Colab seems to be extremely slow).
+An MLP model was trained with the default settings (setting #1), but it failed to learn anything (validation set accuracy = 0.10; no better than random guessing) even after a number of "epochs". Hence it was not trained to completion and the uninformative graph of a horizontal straight line was omitted. Check the MLP portion of the files submitted for more information on the architecture etc. The model and settings were updated a number of times throughout the completion of the assignment.
+In addition, the resulting graphs suggest that most models (with the exception of setting #2) were not trained until the end/to convergence, which is expected since 64000 images translate to only a little more than one full run through the whole dataset (i.e. slightly more than an actual epoch).
+The default settings (SGD with weight and learning rate decay) produced subpar results for all 3 models, presumably because Adam with decent hyperparameters performs significantly better than SGD, in addition to other possible reasons such as the initial learning rate being too high or the weight/learning decay being too aggressive. Using a more adaptive learning rate schedule (reducing learning rate on plateau) may also have improved the performance of the models.
+Due to time constraints, a proper ablation study was not conducted, nor were the models trained to convergence. However, the results roughly align with research results. Early stopping epochs are empirical (i.e. chosen according to best validation set performance despite non-convergence) where it is evident convergence has not occurred.</t>
+  </si>
+  <si>
+    <t>123 (empirical)</t>
+  </si>
+  <si>
+    <t>56.64% (MLP), 74.22% (LeNet5), 90.26% (ResNet32)</t>
+  </si>
+  <si>
+    <t>164, 162, 135 (all empirical)</t>
+  </si>
+  <si>
+    <t>51.38 (MLP), 35.13 (LeNet5), 66.72 (ResNet32)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,6 +231,14 @@
       <family val="2"/>
       <charset val="129"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -167,7 +254,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -258,13 +345,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -295,6 +391,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -304,12 +403,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -464,7 +566,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>Setting #1</a:t>
+            <a:t>Setting #2</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
             <a:latin typeface="백묵 바탕"/>
@@ -547,7 +649,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>Setting #2</a:t>
+            <a:t>Setting #3</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
             <a:latin typeface="백묵 바탕"/>
@@ -630,7 +732,16 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>Setting #3</a:t>
+            <a:t>Setting #4</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" strike="noStrike" spc="-1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> (MLP)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
             <a:latin typeface="백묵 바탕"/>
@@ -640,11 +751,436 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>627739</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>249230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>496796</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114782</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3BB67D6-8F78-4FD2-9F2E-138A94163AC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1281415" y="2453054"/>
+          <a:ext cx="2642513" cy="2330846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>558218</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>228474</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2717840</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>20957</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CEEAFC6-73FB-45A0-9CC4-E660A49E498C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4751086" y="2432298"/>
+          <a:ext cx="3560357" cy="2257777"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>693314</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>192782</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>781300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>170191</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B197781E-F35E-4F88-87BB-675A68A4BDF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9116402" y="2396606"/>
+          <a:ext cx="2674677" cy="2442703"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>354852</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>270810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2723210</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>261472</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF3A4F72-BB30-45D3-BD2D-31E3CA33BAC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13316323" y="2474634"/>
+          <a:ext cx="2368358" cy="2147794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>691029</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>224118</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2263484</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>148878</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A9F1980-405F-418E-9BA0-50580FC4EB35}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13652500" y="2119780"/>
+          <a:ext cx="1572455" cy="232922"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Setting #4 (LeNet5)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
+            <a:latin typeface="백묵 바탕"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>597647</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>270808</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2170102</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>195568</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8A734B4-5A44-4233-BE3A-92774BF4A416}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16883529" y="2166470"/>
+          <a:ext cx="1572455" cy="232922"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Setting #4</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" strike="noStrike" spc="-1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> (ResNet32)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
+            <a:latin typeface="백묵 바탕"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>205443</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>224117</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>119023</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F14526DC-1109-4607-94F0-2677DCAABD1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16491325" y="2427941"/>
+          <a:ext cx="2857500" cy="2360200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -940,149 +1476,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O24"/>
+  <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:O18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="68" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="4" width="12.125" customWidth="1"/>
-    <col min="5" max="5" width="10.125" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
-    <col min="7" max="7" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" customWidth="1"/>
+    <col min="2" max="4" width="12.08203125" customWidth="1"/>
+    <col min="5" max="5" width="10.08203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="37.08203125" customWidth="1"/>
     <col min="8" max="8" width="9.25" customWidth="1"/>
-    <col min="9" max="10" width="12.375" customWidth="1"/>
-    <col min="11" max="11" width="16.125" customWidth="1"/>
-    <col min="12" max="12" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="1026" width="8.625" customWidth="1"/>
+    <col min="9" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.08203125" customWidth="1"/>
+    <col min="12" max="12" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.58203125" customWidth="1"/>
+    <col min="14" max="14" width="33.9140625" customWidth="1"/>
+    <col min="15" max="15" width="46.5" customWidth="1"/>
+    <col min="16" max="1026" width="8.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+    <row r="1" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:15" ht="30.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4">
+        <v>128</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4">
+        <v>128</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="H5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="4">
+        <v>35</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="8"/>
       <c r="E6" s="4">
         <v>128</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="4">
         <v>0.1</v>
@@ -1091,39 +1677,73 @@
         <v>0.9</v>
       </c>
       <c r="K6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4">
+        <v>128</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="G7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1134,270 +1754,414 @@
       <c r="N8" s="6"/>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-    </row>
-    <row r="10" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-    </row>
-    <row r="11" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-    </row>
-    <row r="12" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-    </row>
-    <row r="13" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-    </row>
-    <row r="14" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-    </row>
-    <row r="15" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-    </row>
-    <row r="16" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-    </row>
-    <row r="17" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-    </row>
-    <row r="18" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-    </row>
-    <row r="19" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-    </row>
-    <row r="20" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-    </row>
-    <row r="21" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-    </row>
-    <row r="22" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-    </row>
-    <row r="23" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-    </row>
-    <row r="24" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
+    <row r="9" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+    </row>
+    <row r="10" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+    </row>
+    <row r="11" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+    </row>
+    <row r="12" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+    </row>
+    <row r="13" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+    </row>
+    <row r="14" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+    </row>
+    <row r="15" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+    </row>
+    <row r="16" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+    </row>
+    <row r="17" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+    </row>
+    <row r="18" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+    </row>
+    <row r="19" spans="2:15" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:O18"/>
-    <mergeCell ref="B19:O24"/>
+    <mergeCell ref="B19:O33"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>